<commit_message>
added home timezone to tournament info
</commit_message>
<xml_diff>
--- a/tournaments/2018-mens-world-cup.xlsx
+++ b/tournaments/2018-mens-world-cup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruceo\Documents\code\soccer-tourney-poster\tournaments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/tournaments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB9A5CA-5971-4D9A-8C91-700C785F6DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990D1D99-64D8-3F4F-96FB-3046410F3575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3273" yWindow="3273" windowWidth="19200" windowHeight="10074" activeTab="3" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
+    <workbookView xWindow="3280" yWindow="3280" windowWidth="19200" windowHeight="10080" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tournament" sheetId="8" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="182">
   <si>
     <t>A1</t>
   </si>
@@ -609,6 +609,12 @@
   </si>
   <si>
     <t>pale purple</t>
+  </si>
+  <si>
+    <t>timezone</t>
+  </si>
+  <si>
+    <t>Europe/Moscow</t>
   </si>
 </sst>
 </file>
@@ -702,8 +708,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A35F1197-A800-47A7-9FB8-27BA1E42FC3F}" name="tournament" displayName="tournament" ref="A1:I16" totalsRowShown="0">
-  <autoFilter ref="A1:I16" xr:uid="{A35F1197-A800-47A7-9FB8-27BA1E42FC3F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A35F1197-A800-47A7-9FB8-27BA1E42FC3F}" name="tournament" displayName="tournament" ref="A1:I17" totalsRowShown="0">
+  <autoFilter ref="A1:I17" xr:uid="{A35F1197-A800-47A7-9FB8-27BA1E42FC3F}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A8CDEDD3-FA49-4AD4-8D9F-D3DFCABC2052}" name="key"/>
     <tableColumn id="2" xr3:uid="{88778009-1F1A-4B0F-BCE2-A71F4DD7CF67}" name="en"/>
@@ -770,9 +776,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -810,7 +816,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -916,7 +922,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1058,7 +1064,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1066,29 +1072,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393FFACE-29F0-47F7-B7AD-389E0D6667C5}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.234375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.05859375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.41015625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.3515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.1171875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.76171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.05859375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.46875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -1117,7 +1123,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -1125,7 +1131,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -1154,7 +1160,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -1162,99 +1168,107 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>100</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A6" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>101</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A7" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>102</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A8" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>103</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A9" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>104</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A10" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>105</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A11" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>106</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A12" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>107</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A13" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>135</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A14" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>136</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A15" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>137</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A16" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>138</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>147</v>
       </c>
     </row>
@@ -1276,17 +1290,17 @@
       <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="7.64453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.29296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.46875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5859375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.17578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>62</v>
       </c>
@@ -1321,7 +1335,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1350,7 +1364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1379,7 +1393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1408,7 +1422,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1437,7 +1451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1466,7 +1480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1495,7 +1509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1524,7 +1538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1553,7 +1567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1582,7 +1596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1611,7 +1625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1640,7 +1654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1669,7 +1683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1698,7 +1712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1727,7 +1741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1756,7 +1770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1785,7 +1799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1814,7 +1828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1843,7 +1857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1872,7 +1886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1901,7 +1915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1930,7 +1944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1959,7 +1973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1988,7 +2002,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2017,7 +2031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2046,7 +2060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2075,7 +2089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2104,7 +2118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2133,7 +2147,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2162,7 +2176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2191,7 +2205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2220,7 +2234,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2249,7 +2263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2278,7 +2292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2307,7 +2321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2336,7 +2350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2365,7 +2379,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2394,7 +2408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2423,7 +2437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2452,7 +2466,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2481,7 +2495,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2510,7 +2524,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2539,7 +2553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2568,7 +2582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2597,7 +2611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2626,7 +2640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2655,7 +2669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2684,7 +2698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2713,7 +2727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2742,7 +2756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2771,7 +2785,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2806,7 +2820,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2841,7 +2855,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2870,7 +2884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2899,7 +2913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2928,7 +2942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2963,7 +2977,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2992,7 +3006,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3021,7 +3035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3056,7 +3070,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3085,7 +3099,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3114,7 +3128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3143,7 +3157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3172,7 +3186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3218,9 +3232,9 @@
       <selection activeCell="B2" sqref="B2:B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>66</v>
       </c>
@@ -3228,7 +3242,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3236,7 +3250,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3244,7 +3258,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3252,7 +3266,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3260,7 +3274,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3268,7 +3282,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3276,7 +3290,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3284,7 +3298,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3292,7 +3306,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -3300,7 +3314,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -3308,7 +3322,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -3316,7 +3330,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -3324,7 +3338,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -3332,7 +3346,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -3340,7 +3354,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -3348,7 +3362,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -3356,7 +3370,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -3364,7 +3378,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -3372,7 +3386,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -3380,7 +3394,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -3388,7 +3402,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -3396,7 +3410,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -3404,7 +3418,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -3412,7 +3426,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -3420,7 +3434,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -3428,7 +3442,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -3436,7 +3450,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -3444,7 +3458,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -3452,7 +3466,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -3460,7 +3474,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -3468,7 +3482,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -3476,7 +3490,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>27</v>
       </c>
@@ -3497,16 +3511,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC88D2E7-F4E0-42E8-919E-CAB4A74488F8}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="10" max="10" width="12.1171875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -3538,7 +3552,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>156</v>
       </c>
@@ -3549,7 +3563,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>159</v>
       </c>
@@ -3560,7 +3574,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>162</v>
       </c>
@@ -3571,7 +3585,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>165</v>
       </c>
@@ -3582,7 +3596,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>168</v>
       </c>
@@ -3593,7 +3607,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>171</v>
       </c>
@@ -3604,7 +3618,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>174</v>
       </c>
@@ -3615,7 +3629,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>177</v>
       </c>

</xml_diff>